<commit_message>
Rename repo, add files
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -1,39 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/music/H-Con-Sabor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/dev/h-con-sabor-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA52318C-38DD-B646-9EFE-E5C1EDA1033F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7669E05F-9EE6-1F41-B7DB-74BE96DA84AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1740" yWindow="460" windowWidth="19040" windowHeight="15540" xr2:uid="{74CF8044-3979-624F-B98D-1F70AF4C8FD5}"/>
+    <workbookView xWindow="6700" yWindow="460" windowWidth="19040" windowHeight="15540" activeTab="1" xr2:uid="{74CF8044-3979-624F-B98D-1F70AF4C8FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>Anacaona</t>
   </si>
@@ -120,13 +113,16 @@
   </si>
   <si>
     <t>Yesterday</t>
+  </si>
+  <si>
+    <t>title:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +140,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Terminal"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,10 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,187 +489,187 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C0E305-8EA4-9049-B579-C7FA70E513C3}">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="56.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -674,4 +677,310 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB67B21-D624-7E4E-85AF-EA169FC8CF7C}">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="39.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:B46">
+    <sortCondition ref="B1:B46"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>